<commit_message>
Move logic to higher level
</commit_message>
<xml_diff>
--- a/test/data/duplicate-headers.xlsx
+++ b/test/data/duplicate-headers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eirik/Development/private/tech.ml.dataset/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712D494F-DE0E-924E-B8BE-3EB4EACA38DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E298B6AB-64F4-4C4D-A951-420B74B08324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{062F8BAC-300C-A54C-9E7B-D3240CE3FBF8}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>